<commit_message>
Changes in pie chart made
</commit_message>
<xml_diff>
--- a/croc_project.xlsx
+++ b/croc_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Charlie/Desktop/School/Data_Science/Projects/Excel_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Charlie/Desktop/School/Data_Science/Projects/Excel_project/excel_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84914241-1C01-004E-BEB5-8ECF1B83823D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D283826-39BD-7B40-8DF6-D1DACD093D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{EEE10FFB-FA0C-874A-91AF-A269BE40C7EC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId3"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -9968,10 +9968,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="105"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="5"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
@@ -9986,11 +9986,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -10018,11 +10018,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -10039,54 +10039,51 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:gradFill rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="110000"/>
-                  <a:satMod val="105000"/>
-                  <a:tint val="67000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="50000">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="103000"/>
-                  <a:tint val="73000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="109000"/>
-                  <a:tint val="81000"/>
-                </a:schemeClr>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="5400000" scaled="0"/>
-          </a:gradFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:shade val="95000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
         <c:marker>
           <c:symbol val="circle"/>
-          <c:size val="4"/>
+          <c:size val="6"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:spPr>
-            <a:noFill/>
+            <a:pattFill prst="pct75">
+              <a:fgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:sysClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:txPr>
             <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -10095,12 +10092,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="lt1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -10110,7 +10104,7 @@
               <a:endParaRPr lang="en-ES"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="inEnd"/>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="1"/>
@@ -10125,121 +10119,59 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
-          <a:gradFill rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="110000"/>
-                  <a:satMod val="105000"/>
-                  <a:tint val="67000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="50000">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="103000"/>
-                  <a:tint val="73000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="109000"/>
-                  <a:tint val="81000"/>
-                </a:schemeClr>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="5400000" scaled="0"/>
-          </a:gradFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:shade val="95000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:shade val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
-          <a:gradFill rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="110000"/>
-                  <a:satMod val="105000"/>
-                  <a:tint val="67000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="50000">
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="103000"/>
-                  <a:tint val="73000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="109000"/>
-                  <a:tint val="81000"/>
-                </a:schemeClr>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="5400000" scaled="0"/>
-          </a:gradFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:shade val="95000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
-          <a:gradFill rotWithShape="1">
-            <a:gsLst>
-              <a:gs pos="0">
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="110000"/>
-                  <a:satMod val="105000"/>
-                  <a:tint val="67000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="50000">
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="103000"/>
-                  <a:tint val="73000"/>
-                </a:schemeClr>
-              </a:gs>
-              <a:gs pos="100000">
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="105000"/>
-                  <a:satMod val="109000"/>
-                  <a:tint val="81000"/>
-                </a:schemeClr>
-              </a:gs>
-            </a:gsLst>
-            <a:lin ang="5400000" scaled="0"/>
-          </a:gradFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:shade val="95000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:tint val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -10265,41 +10197,21 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="110000"/>
-                      <a:satMod val="105000"/>
-                      <a:tint val="67000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="103000"/>
-                      <a:tint val="73000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="109000"/>
-                      <a:tint val="81000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -10311,41 +10223,19 @@
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="110000"/>
-                      <a:satMod val="105000"/>
-                      <a:tint val="67000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="103000"/>
-                      <a:tint val="73000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="109000"/>
-                      <a:tint val="81000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:shade val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -10357,41 +10247,21 @@
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="110000"/>
-                      <a:satMod val="105000"/>
-                      <a:tint val="67000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="103000"/>
-                      <a:tint val="73000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="109000"/>
-                      <a:tint val="81000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:shade val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:tint val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -10401,11 +10271,30 @@
           </c:dPt>
           <c:dLbls>
             <c:spPr>
-              <a:noFill/>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:sysClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:bgClr>
+              </a:pattFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -10414,12 +10303,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="lt1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10429,7 +10315,7 @@
                 <a:endParaRPr lang="en-ES"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="1"/>
@@ -10441,9 +10327,9 @@
               <c:spPr>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
                     </a:schemeClr>
                   </a:solidFill>
                 </a:ln>
@@ -10496,7 +10382,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -10519,7 +10405,12 @@
       <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -10532,9 +10423,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -10558,14 +10449,30 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -11717,39 +11624,8 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent5"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -12291,43 +12167,43 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -12335,14 +12211,30 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12355,122 +12247,155 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
           <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="2">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr/>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="15875" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
@@ -12489,17 +12414,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -12516,15 +12441,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -12540,7 +12465,7 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -12559,11 +12484,12 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -12584,12 +12510,24 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -12603,12 +12541,24 @@
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -12622,9 +12572,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -12641,9 +12591,9 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -12654,14 +12604,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -12669,7 +12627,7 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -12682,17 +12640,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12710,12 +12668,12 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -12724,24 +12682,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="2"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -12753,9 +12711,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -12773,9 +12731,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -12786,11 +12744,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -33443,7 +33406,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20B6C053-13E0-7241-A8D3-4E83E09BC858}" name="avg_length_species" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Species">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20B6C053-13E0-7241-A8D3-4E83E09BC858}" name="avg_length_species" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Species">
   <location ref="A41:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -33976,7 +33939,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9BA5ABC-D0BD-254A-B014-0D326FA826D0}" name="count by genus" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Genus">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9BA5ABC-D0BD-254A-B014-0D326FA826D0}" name="count by genus" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Genus">
   <location ref="A26:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0">
@@ -35090,7 +35053,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16800E7F-174B-0941-AC4A-45AEB857E302}" name="species_count" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Species">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16800E7F-174B-0941-AC4A-45AEB857E302}" name="species_count" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Species">
   <location ref="A3:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -35224,7 +35187,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6DE011A0-5DAC-DE4E-B770-4F7DC6E6C97A}" name="avg_weight_species" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Species">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6DE011A0-5DAC-DE4E-B770-4F7DC6E6C97A}" name="avg_weight_species" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Species">
   <location ref="A65:B84" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -86829,8 +86792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0EEB4D-0759-9640-9CF7-00A0D61D5ADD}">
   <dimension ref="A3:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="106" zoomScaleNormal="206" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" zoomScaleNormal="206" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Explanation to some outliers
</commit_message>
<xml_diff>
--- a/croc_project.xlsx
+++ b/croc_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Charlie/Desktop/School/Data_Science/Projects/Excel_project/excel_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D283826-39BD-7B40-8DF6-D1DACD093D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C34A5A-3746-6B4F-AF1D-0B41FDA97106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{EEE10FFB-FA0C-874A-91AF-A269BE40C7EC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,6 +42,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1408B32F-EACE-B54F-A263-FA3DBC36148C}</author>
+  </authors>
+  <commentList>
+    <comment ref="M59" authorId="0" shapeId="0" xr:uid="{1408B32F-EACE-B54F-A263-FA3DBC36148C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Both Crocodiles porosus and Crocodylus niloticus seem to be outliers. On further investigation I’ve been able to confirm that those numbers are correct and that they are usually bigger and heavier than other species.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{F8F7AF23-C46A-AF4C-A073-B6656B73E185}" keepAlive="1" name="Query - crocodile_dataset" description="Connection to the 'crocodile_dataset' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
@@ -9278,7 +9296,7 @@
     <t>Average of Observed Weight (kg)</t>
   </si>
   <si>
-    <t>g</t>
+    <t xml:space="preserve">Differences </t>
   </si>
 </sst>
 </file>
@@ -9288,7 +9306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9296,16 +9314,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -9313,11 +9350,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -9329,6 +9381,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10054,8 +10107,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -13922,6 +13974,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="carlos ramirez" id="{09CB50DF-FC12-2C48-8902-835225B18043}" userId="2044dc370084a43d" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Carlos Javier Ramirez Kunja" refreshedDate="45921.939378124996" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1000" xr:uid="{10442531-3E18-2747-93FC-0044896BF37C}">
   <cacheSource type="worksheet">
@@ -33406,540 +33464,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20B6C053-13E0-7241-A8D3-4E83E09BC858}" name="avg_length_species" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Species">
-  <location ref="A41:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="19">
-        <item x="1"/>
-        <item x="17"/>
-        <item x="2"/>
-        <item x="15"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="13"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="11"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="14"/>
-        <item x="16"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="2" showAll="0">
-      <items count="391">
-        <item x="361"/>
-        <item x="232"/>
-        <item x="123"/>
-        <item x="335"/>
-        <item x="382"/>
-        <item x="327"/>
-        <item x="228"/>
-        <item x="292"/>
-        <item x="284"/>
-        <item x="289"/>
-        <item x="40"/>
-        <item x="306"/>
-        <item x="163"/>
-        <item x="25"/>
-        <item x="7"/>
-        <item x="133"/>
-        <item x="313"/>
-        <item x="184"/>
-        <item x="298"/>
-        <item x="301"/>
-        <item x="50"/>
-        <item x="252"/>
-        <item x="303"/>
-        <item x="254"/>
-        <item x="260"/>
-        <item x="144"/>
-        <item x="250"/>
-        <item x="153"/>
-        <item x="288"/>
-        <item x="190"/>
-        <item x="125"/>
-        <item x="227"/>
-        <item x="246"/>
-        <item x="231"/>
-        <item x="336"/>
-        <item x="274"/>
-        <item x="328"/>
-        <item x="221"/>
-        <item x="344"/>
-        <item x="32"/>
-        <item x="237"/>
-        <item x="74"/>
-        <item x="323"/>
-        <item x="340"/>
-        <item x="171"/>
-        <item x="240"/>
-        <item x="102"/>
-        <item x="146"/>
-        <item x="120"/>
-        <item x="229"/>
-        <item x="277"/>
-        <item x="389"/>
-        <item x="161"/>
-        <item x="126"/>
-        <item x="367"/>
-        <item x="47"/>
-        <item x="296"/>
-        <item x="354"/>
-        <item x="150"/>
-        <item x="149"/>
-        <item x="31"/>
-        <item x="145"/>
-        <item x="136"/>
-        <item x="36"/>
-        <item x="264"/>
-        <item x="18"/>
-        <item x="2"/>
-        <item x="230"/>
-        <item x="70"/>
-        <item x="205"/>
-        <item x="138"/>
-        <item x="132"/>
-        <item x="365"/>
-        <item x="359"/>
-        <item x="312"/>
-        <item x="54"/>
-        <item x="62"/>
-        <item x="82"/>
-        <item x="10"/>
-        <item x="75"/>
-        <item x="182"/>
-        <item x="57"/>
-        <item x="357"/>
-        <item x="197"/>
-        <item x="322"/>
-        <item x="338"/>
-        <item x="201"/>
-        <item x="14"/>
-        <item x="272"/>
-        <item x="213"/>
-        <item x="209"/>
-        <item x="203"/>
-        <item x="104"/>
-        <item x="334"/>
-        <item x="168"/>
-        <item x="356"/>
-        <item x="179"/>
-        <item x="278"/>
-        <item x="177"/>
-        <item x="117"/>
-        <item x="34"/>
-        <item x="135"/>
-        <item x="157"/>
-        <item x="109"/>
-        <item x="119"/>
-        <item x="266"/>
-        <item x="19"/>
-        <item x="189"/>
-        <item x="110"/>
-        <item x="244"/>
-        <item x="97"/>
-        <item x="72"/>
-        <item x="239"/>
-        <item x="317"/>
-        <item x="208"/>
-        <item x="162"/>
-        <item x="247"/>
-        <item x="215"/>
-        <item x="280"/>
-        <item x="68"/>
-        <item x="341"/>
-        <item x="358"/>
-        <item x="217"/>
-        <item x="173"/>
-        <item x="219"/>
-        <item x="199"/>
-        <item x="22"/>
-        <item x="198"/>
-        <item x="169"/>
-        <item x="351"/>
-        <item x="304"/>
-        <item x="245"/>
-        <item x="156"/>
-        <item x="11"/>
-        <item x="60"/>
-        <item x="222"/>
-        <item x="286"/>
-        <item x="175"/>
-        <item x="253"/>
-        <item x="0"/>
-        <item x="248"/>
-        <item x="167"/>
-        <item x="56"/>
-        <item x="112"/>
-        <item x="268"/>
-        <item x="81"/>
-        <item x="324"/>
-        <item x="16"/>
-        <item x="176"/>
-        <item x="15"/>
-        <item x="143"/>
-        <item x="200"/>
-        <item x="164"/>
-        <item x="29"/>
-        <item x="51"/>
-        <item x="211"/>
-        <item x="108"/>
-        <item x="193"/>
-        <item x="267"/>
-        <item x="142"/>
-        <item x="256"/>
-        <item x="353"/>
-        <item x="67"/>
-        <item x="178"/>
-        <item x="66"/>
-        <item x="258"/>
-        <item x="118"/>
-        <item x="147"/>
-        <item x="269"/>
-        <item x="87"/>
-        <item x="127"/>
-        <item x="58"/>
-        <item x="285"/>
-        <item x="154"/>
-        <item x="33"/>
-        <item x="89"/>
-        <item x="92"/>
-        <item x="202"/>
-        <item x="314"/>
-        <item x="73"/>
-        <item x="310"/>
-        <item x="41"/>
-        <item x="261"/>
-        <item x="295"/>
-        <item x="114"/>
-        <item x="388"/>
-        <item x="368"/>
-        <item x="308"/>
-        <item x="85"/>
-        <item x="249"/>
-        <item x="3"/>
-        <item x="45"/>
-        <item x="23"/>
-        <item x="78"/>
-        <item x="95"/>
-        <item x="339"/>
-        <item x="207"/>
-        <item x="346"/>
-        <item x="42"/>
-        <item x="46"/>
-        <item x="20"/>
-        <item x="325"/>
-        <item x="65"/>
-        <item x="265"/>
-        <item x="53"/>
-        <item x="94"/>
-        <item x="90"/>
-        <item x="224"/>
-        <item x="242"/>
-        <item x="160"/>
-        <item x="271"/>
-        <item x="12"/>
-        <item x="5"/>
-        <item x="366"/>
-        <item x="257"/>
-        <item x="195"/>
-        <item x="192"/>
-        <item x="103"/>
-        <item x="83"/>
-        <item x="86"/>
-        <item x="37"/>
-        <item x="216"/>
-        <item x="148"/>
-        <item x="129"/>
-        <item x="77"/>
-        <item x="165"/>
-        <item x="166"/>
-        <item x="137"/>
-        <item x="181"/>
-        <item x="111"/>
-        <item x="76"/>
-        <item x="319"/>
-        <item x="387"/>
-        <item x="6"/>
-        <item x="183"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="151"/>
-        <item x="63"/>
-        <item x="263"/>
-        <item x="212"/>
-        <item x="91"/>
-        <item x="174"/>
-        <item x="225"/>
-        <item x="35"/>
-        <item x="49"/>
-        <item x="140"/>
-        <item x="170"/>
-        <item x="220"/>
-        <item x="276"/>
-        <item x="71"/>
-        <item x="236"/>
-        <item x="43"/>
-        <item x="8"/>
-        <item x="188"/>
-        <item x="93"/>
-        <item x="84"/>
-        <item x="159"/>
-        <item x="128"/>
-        <item x="113"/>
-        <item x="251"/>
-        <item x="121"/>
-        <item x="172"/>
-        <item x="206"/>
-        <item x="371"/>
-        <item x="348"/>
-        <item x="24"/>
-        <item x="105"/>
-        <item x="384"/>
-        <item x="27"/>
-        <item x="362"/>
-        <item x="369"/>
-        <item x="38"/>
-        <item x="352"/>
-        <item x="122"/>
-        <item x="233"/>
-        <item x="347"/>
-        <item x="218"/>
-        <item x="79"/>
-        <item x="355"/>
-        <item x="259"/>
-        <item x="320"/>
-        <item x="9"/>
-        <item x="44"/>
-        <item x="116"/>
-        <item x="321"/>
-        <item x="281"/>
-        <item x="255"/>
-        <item x="360"/>
-        <item x="326"/>
-        <item x="364"/>
-        <item x="226"/>
-        <item x="186"/>
-        <item x="279"/>
-        <item x="187"/>
-        <item x="180"/>
-        <item x="185"/>
-        <item x="39"/>
-        <item x="152"/>
-        <item x="96"/>
-        <item x="376"/>
-        <item x="291"/>
-        <item x="210"/>
-        <item x="350"/>
-        <item x="13"/>
-        <item x="59"/>
-        <item x="385"/>
-        <item x="115"/>
-        <item x="290"/>
-        <item x="139"/>
-        <item x="318"/>
-        <item x="378"/>
-        <item x="270"/>
-        <item x="4"/>
-        <item x="287"/>
-        <item x="55"/>
-        <item x="342"/>
-        <item x="349"/>
-        <item x="223"/>
-        <item x="275"/>
-        <item x="131"/>
-        <item x="273"/>
-        <item x="80"/>
-        <item x="307"/>
-        <item x="262"/>
-        <item x="26"/>
-        <item x="294"/>
-        <item x="381"/>
-        <item x="331"/>
-        <item x="191"/>
-        <item x="383"/>
-        <item x="329"/>
-        <item x="343"/>
-        <item x="241"/>
-        <item x="1"/>
-        <item x="238"/>
-        <item x="30"/>
-        <item x="363"/>
-        <item x="234"/>
-        <item x="300"/>
-        <item x="196"/>
-        <item x="134"/>
-        <item x="283"/>
-        <item x="374"/>
-        <item x="299"/>
-        <item x="330"/>
-        <item x="311"/>
-        <item x="214"/>
-        <item x="64"/>
-        <item x="305"/>
-        <item x="17"/>
-        <item x="345"/>
-        <item x="293"/>
-        <item x="316"/>
-        <item x="370"/>
-        <item x="386"/>
-        <item x="333"/>
-        <item x="377"/>
-        <item x="100"/>
-        <item x="155"/>
-        <item x="21"/>
-        <item x="98"/>
-        <item x="315"/>
-        <item x="28"/>
-        <item x="337"/>
-        <item x="235"/>
-        <item x="375"/>
-        <item x="372"/>
-        <item x="379"/>
-        <item x="88"/>
-        <item x="61"/>
-        <item x="204"/>
-        <item x="309"/>
-        <item x="332"/>
-        <item x="69"/>
-        <item x="99"/>
-        <item x="380"/>
-        <item x="194"/>
-        <item x="373"/>
-        <item x="101"/>
-        <item x="282"/>
-        <item x="141"/>
-        <item x="302"/>
-        <item x="52"/>
-        <item x="130"/>
-        <item x="297"/>
-        <item x="48"/>
-        <item x="158"/>
-        <item x="124"/>
-        <item x="243"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="49" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Observed Length (m)" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9BA5ABC-D0BD-254A-B014-0D326FA826D0}" name="count by genus" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Genus">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A9BA5ABC-D0BD-254A-B014-0D326FA826D0}" name="count by genus" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Genus">
   <location ref="A26:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0">
@@ -35052,8 +34577,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16800E7F-174B-0941-AC4A-45AEB857E302}" name="species_count" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Species">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16800E7F-174B-0941-AC4A-45AEB857E302}" name="species_count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Species">
   <location ref="A3:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -35186,8 +34711,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6DE011A0-5DAC-DE4E-B770-4F7DC6E6C97A}" name="avg_weight_species" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Species">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6DE011A0-5DAC-DE4E-B770-4F7DC6E6C97A}" name="avg_weight_species" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3" rowHeaderCaption="Species">
   <location ref="A65:B84" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -35296,6 +34821,539 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Average of Observed Weight (kg)" fld="6" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20B6C053-13E0-7241-A8D3-4E83E09BC858}" name="avg_length_species" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Species">
+  <location ref="A41:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="19">
+        <item x="1"/>
+        <item x="17"/>
+        <item x="2"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="14"/>
+        <item x="16"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0">
+      <items count="391">
+        <item x="361"/>
+        <item x="232"/>
+        <item x="123"/>
+        <item x="335"/>
+        <item x="382"/>
+        <item x="327"/>
+        <item x="228"/>
+        <item x="292"/>
+        <item x="284"/>
+        <item x="289"/>
+        <item x="40"/>
+        <item x="306"/>
+        <item x="163"/>
+        <item x="25"/>
+        <item x="7"/>
+        <item x="133"/>
+        <item x="313"/>
+        <item x="184"/>
+        <item x="298"/>
+        <item x="301"/>
+        <item x="50"/>
+        <item x="252"/>
+        <item x="303"/>
+        <item x="254"/>
+        <item x="260"/>
+        <item x="144"/>
+        <item x="250"/>
+        <item x="153"/>
+        <item x="288"/>
+        <item x="190"/>
+        <item x="125"/>
+        <item x="227"/>
+        <item x="246"/>
+        <item x="231"/>
+        <item x="336"/>
+        <item x="274"/>
+        <item x="328"/>
+        <item x="221"/>
+        <item x="344"/>
+        <item x="32"/>
+        <item x="237"/>
+        <item x="74"/>
+        <item x="323"/>
+        <item x="340"/>
+        <item x="171"/>
+        <item x="240"/>
+        <item x="102"/>
+        <item x="146"/>
+        <item x="120"/>
+        <item x="229"/>
+        <item x="277"/>
+        <item x="389"/>
+        <item x="161"/>
+        <item x="126"/>
+        <item x="367"/>
+        <item x="47"/>
+        <item x="296"/>
+        <item x="354"/>
+        <item x="150"/>
+        <item x="149"/>
+        <item x="31"/>
+        <item x="145"/>
+        <item x="136"/>
+        <item x="36"/>
+        <item x="264"/>
+        <item x="18"/>
+        <item x="2"/>
+        <item x="230"/>
+        <item x="70"/>
+        <item x="205"/>
+        <item x="138"/>
+        <item x="132"/>
+        <item x="365"/>
+        <item x="359"/>
+        <item x="312"/>
+        <item x="54"/>
+        <item x="62"/>
+        <item x="82"/>
+        <item x="10"/>
+        <item x="75"/>
+        <item x="182"/>
+        <item x="57"/>
+        <item x="357"/>
+        <item x="197"/>
+        <item x="322"/>
+        <item x="338"/>
+        <item x="201"/>
+        <item x="14"/>
+        <item x="272"/>
+        <item x="213"/>
+        <item x="209"/>
+        <item x="203"/>
+        <item x="104"/>
+        <item x="334"/>
+        <item x="168"/>
+        <item x="356"/>
+        <item x="179"/>
+        <item x="278"/>
+        <item x="177"/>
+        <item x="117"/>
+        <item x="34"/>
+        <item x="135"/>
+        <item x="157"/>
+        <item x="109"/>
+        <item x="119"/>
+        <item x="266"/>
+        <item x="19"/>
+        <item x="189"/>
+        <item x="110"/>
+        <item x="244"/>
+        <item x="97"/>
+        <item x="72"/>
+        <item x="239"/>
+        <item x="317"/>
+        <item x="208"/>
+        <item x="162"/>
+        <item x="247"/>
+        <item x="215"/>
+        <item x="280"/>
+        <item x="68"/>
+        <item x="341"/>
+        <item x="358"/>
+        <item x="217"/>
+        <item x="173"/>
+        <item x="219"/>
+        <item x="199"/>
+        <item x="22"/>
+        <item x="198"/>
+        <item x="169"/>
+        <item x="351"/>
+        <item x="304"/>
+        <item x="245"/>
+        <item x="156"/>
+        <item x="11"/>
+        <item x="60"/>
+        <item x="222"/>
+        <item x="286"/>
+        <item x="175"/>
+        <item x="253"/>
+        <item x="0"/>
+        <item x="248"/>
+        <item x="167"/>
+        <item x="56"/>
+        <item x="112"/>
+        <item x="268"/>
+        <item x="81"/>
+        <item x="324"/>
+        <item x="16"/>
+        <item x="176"/>
+        <item x="15"/>
+        <item x="143"/>
+        <item x="200"/>
+        <item x="164"/>
+        <item x="29"/>
+        <item x="51"/>
+        <item x="211"/>
+        <item x="108"/>
+        <item x="193"/>
+        <item x="267"/>
+        <item x="142"/>
+        <item x="256"/>
+        <item x="353"/>
+        <item x="67"/>
+        <item x="178"/>
+        <item x="66"/>
+        <item x="258"/>
+        <item x="118"/>
+        <item x="147"/>
+        <item x="269"/>
+        <item x="87"/>
+        <item x="127"/>
+        <item x="58"/>
+        <item x="285"/>
+        <item x="154"/>
+        <item x="33"/>
+        <item x="89"/>
+        <item x="92"/>
+        <item x="202"/>
+        <item x="314"/>
+        <item x="73"/>
+        <item x="310"/>
+        <item x="41"/>
+        <item x="261"/>
+        <item x="295"/>
+        <item x="114"/>
+        <item x="388"/>
+        <item x="368"/>
+        <item x="308"/>
+        <item x="85"/>
+        <item x="249"/>
+        <item x="3"/>
+        <item x="45"/>
+        <item x="23"/>
+        <item x="78"/>
+        <item x="95"/>
+        <item x="339"/>
+        <item x="207"/>
+        <item x="346"/>
+        <item x="42"/>
+        <item x="46"/>
+        <item x="20"/>
+        <item x="325"/>
+        <item x="65"/>
+        <item x="265"/>
+        <item x="53"/>
+        <item x="94"/>
+        <item x="90"/>
+        <item x="224"/>
+        <item x="242"/>
+        <item x="160"/>
+        <item x="271"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="366"/>
+        <item x="257"/>
+        <item x="195"/>
+        <item x="192"/>
+        <item x="103"/>
+        <item x="83"/>
+        <item x="86"/>
+        <item x="37"/>
+        <item x="216"/>
+        <item x="148"/>
+        <item x="129"/>
+        <item x="77"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="137"/>
+        <item x="181"/>
+        <item x="111"/>
+        <item x="76"/>
+        <item x="319"/>
+        <item x="387"/>
+        <item x="6"/>
+        <item x="183"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="151"/>
+        <item x="63"/>
+        <item x="263"/>
+        <item x="212"/>
+        <item x="91"/>
+        <item x="174"/>
+        <item x="225"/>
+        <item x="35"/>
+        <item x="49"/>
+        <item x="140"/>
+        <item x="170"/>
+        <item x="220"/>
+        <item x="276"/>
+        <item x="71"/>
+        <item x="236"/>
+        <item x="43"/>
+        <item x="8"/>
+        <item x="188"/>
+        <item x="93"/>
+        <item x="84"/>
+        <item x="159"/>
+        <item x="128"/>
+        <item x="113"/>
+        <item x="251"/>
+        <item x="121"/>
+        <item x="172"/>
+        <item x="206"/>
+        <item x="371"/>
+        <item x="348"/>
+        <item x="24"/>
+        <item x="105"/>
+        <item x="384"/>
+        <item x="27"/>
+        <item x="362"/>
+        <item x="369"/>
+        <item x="38"/>
+        <item x="352"/>
+        <item x="122"/>
+        <item x="233"/>
+        <item x="347"/>
+        <item x="218"/>
+        <item x="79"/>
+        <item x="355"/>
+        <item x="259"/>
+        <item x="320"/>
+        <item x="9"/>
+        <item x="44"/>
+        <item x="116"/>
+        <item x="321"/>
+        <item x="281"/>
+        <item x="255"/>
+        <item x="360"/>
+        <item x="326"/>
+        <item x="364"/>
+        <item x="226"/>
+        <item x="186"/>
+        <item x="279"/>
+        <item x="187"/>
+        <item x="180"/>
+        <item x="185"/>
+        <item x="39"/>
+        <item x="152"/>
+        <item x="96"/>
+        <item x="376"/>
+        <item x="291"/>
+        <item x="210"/>
+        <item x="350"/>
+        <item x="13"/>
+        <item x="59"/>
+        <item x="385"/>
+        <item x="115"/>
+        <item x="290"/>
+        <item x="139"/>
+        <item x="318"/>
+        <item x="378"/>
+        <item x="270"/>
+        <item x="4"/>
+        <item x="287"/>
+        <item x="55"/>
+        <item x="342"/>
+        <item x="349"/>
+        <item x="223"/>
+        <item x="275"/>
+        <item x="131"/>
+        <item x="273"/>
+        <item x="80"/>
+        <item x="307"/>
+        <item x="262"/>
+        <item x="26"/>
+        <item x="294"/>
+        <item x="381"/>
+        <item x="331"/>
+        <item x="191"/>
+        <item x="383"/>
+        <item x="329"/>
+        <item x="343"/>
+        <item x="241"/>
+        <item x="1"/>
+        <item x="238"/>
+        <item x="30"/>
+        <item x="363"/>
+        <item x="234"/>
+        <item x="300"/>
+        <item x="196"/>
+        <item x="134"/>
+        <item x="283"/>
+        <item x="374"/>
+        <item x="299"/>
+        <item x="330"/>
+        <item x="311"/>
+        <item x="214"/>
+        <item x="64"/>
+        <item x="305"/>
+        <item x="17"/>
+        <item x="345"/>
+        <item x="293"/>
+        <item x="316"/>
+        <item x="370"/>
+        <item x="386"/>
+        <item x="333"/>
+        <item x="377"/>
+        <item x="100"/>
+        <item x="155"/>
+        <item x="21"/>
+        <item x="98"/>
+        <item x="315"/>
+        <item x="28"/>
+        <item x="337"/>
+        <item x="235"/>
+        <item x="375"/>
+        <item x="372"/>
+        <item x="379"/>
+        <item x="88"/>
+        <item x="61"/>
+        <item x="204"/>
+        <item x="309"/>
+        <item x="332"/>
+        <item x="69"/>
+        <item x="99"/>
+        <item x="380"/>
+        <item x="194"/>
+        <item x="373"/>
+        <item x="101"/>
+        <item x="282"/>
+        <item x="141"/>
+        <item x="302"/>
+        <item x="52"/>
+        <item x="130"/>
+        <item x="297"/>
+        <item x="48"/>
+        <item x="158"/>
+        <item x="124"/>
+        <item x="243"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="49" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Observed Length (m)" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
     <format dxfId="2">
@@ -35692,12 +35750,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="M59" dT="2025-09-25T19:42:03.19" personId="{09CB50DF-FC12-2C48-8902-835225B18043}" id="{1408B32F-EACE-B54F-A263-FA3DBC36148C}">
+    <text>Both Crocodiles porosus and Crocodylus niloticus seem to be outliers. On further investigation I’ve been able to confirm that those numbers are correct and that they are usually bigger and heavier than other species.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4938BC-38B9-2245-A707-6DCAC973F1B8}">
   <dimension ref="A1:U1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35820,9 +35886,7 @@
         <f>COUNTBLANK(crocodile_dataset[[Observation ID]:[Notes]])</f>
         <v>0</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>3075</v>
-      </c>
+      <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -86789,11 +86853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0EEB4D-0759-9640-9CF7-00A0D61D5ADD}">
-  <dimension ref="A3:B84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0EEB4D-0759-9640-9CF7-00A0D61D5ADD}">
+  <dimension ref="A3:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" zoomScaleNormal="206" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="75" zoomScaleNormal="206" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -87084,7 +87148,7 @@
         <v>3.6666666666666665</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>189</v>
       </c>
@@ -87092,7 +87156,7 @@
         <v>2.1454411764705879</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -87100,7 +87164,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>128</v>
       </c>
@@ -87108,7 +87172,7 @@
         <v>4.4077586206896555</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>121</v>
       </c>
@@ -87116,7 +87180,7 @@
         <v>2.5176119402985075</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>146</v>
       </c>
@@ -87124,7 +87188,7 @@
         <v>2.3179661016949145</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>60</v>
       </c>
@@ -87132,7 +87196,7 @@
         <v>2.1564444444444448</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>77</v>
       </c>
@@ -87140,7 +87204,7 @@
         <v>2.3355769230769234</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>202</v>
       </c>
@@ -87148,7 +87212,7 @@
         <v>2.4716363636363634</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>321</v>
       </c>
@@ -87156,7 +87220,7 @@
         <v>1.9958928571428569</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>68</v>
       </c>
@@ -87164,15 +87228,18 @@
         <v>1.22875</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B59" s="8">
         <v>1.1203508771929824</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="M59" s="9" t="s">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>3069</v>
       </c>
@@ -87343,6 +87410,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>